<commit_message>
split servoCtrl -> servoDataCtrl and servoMotionCtrl
</commit_message>
<xml_diff>
--- a/Calculations and Definitions/Geschwindigkeit fuer Servos.xlsx
+++ b/Calculations and Definitions/Geschwindigkeit fuer Servos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\JujuBot_uC_A8\Calculations and Definitions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5866495F-A987-42FC-8B34-7CF6BFEBB763}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55BAA912-7050-4991-9D7F-A731CE9B0D6D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="12220" windowHeight="17760" activeTab="2" xr2:uid="{75FC373F-61E7-46CB-9D88-857622E45D35}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="83">
   <si>
     <t>MG90S</t>
   </si>
@@ -84,18 +84,6 @@
   </si>
   <si>
     <t>[1 Step/ x ms]</t>
-  </si>
-  <si>
-    <t>Look Up Table</t>
-  </si>
-  <si>
-    <t>Sollwert</t>
-  </si>
-  <si>
-    <t>delta Steps</t>
-  </si>
-  <si>
-    <t>delta Cyles</t>
   </si>
   <si>
     <t>f [1/s]</t>
@@ -528,6 +516,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -543,13 +538,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -20533,8 +20521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80FAD0B1-6266-4141-8BE4-85A9D5BCF6C5}">
   <dimension ref="A1:R107"/>
   <sheetViews>
-    <sheetView topLeftCell="B19" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A24" sqref="A24:I67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -20553,7 +20541,7 @@
         <v>0</v>
       </c>
       <c r="N1" s="7" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.35">
@@ -20570,15 +20558,15 @@
         <v>10</v>
       </c>
       <c r="N2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="O2" s="3">
         <v>2</v>
       </c>
-      <c r="Q2" s="40" t="s">
-        <v>33</v>
-      </c>
-      <c r="R2" s="40"/>
+      <c r="Q2" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="R2" s="43"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" s="4">
@@ -20594,16 +20582,16 @@
         <v>410</v>
       </c>
       <c r="N3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="O3" s="3">
         <f>O2*360</f>
         <v>720</v>
       </c>
-      <c r="Q3" s="39" t="s">
-        <v>32</v>
-      </c>
-      <c r="R3" s="39"/>
+      <c r="Q3" s="42" t="s">
+        <v>28</v>
+      </c>
+      <c r="R3" s="42"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
@@ -20620,7 +20608,7 @@
         <v>400</v>
       </c>
       <c r="N4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="O4" s="3">
         <f>O2*$E$5</f>
@@ -20636,7 +20624,7 @@
         <v>800</v>
       </c>
       <c r="P5" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="Q5" s="1">
         <v>20</v>
@@ -20663,22 +20651,22 @@
         <v>16</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="N7" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="O7" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="P7" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="Q7" s="3" t="s">
         <v>9</v>
       </c>
       <c r="R7" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.35">
@@ -20775,10 +20763,10 @@
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A11" s="41" t="s">
-        <v>36</v>
-      </c>
-      <c r="B11" s="41"/>
+      <c r="A11" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="44"/>
       <c r="N11">
         <f t="shared" si="4"/>
         <v>0.04</v>
@@ -20831,10 +20819,10 @@
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A13" s="41" t="s">
+      <c r="A13" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="41"/>
+      <c r="B13" s="44"/>
       <c r="N13">
         <f t="shared" si="4"/>
         <v>6.0000000000000005E-2</v>
@@ -20861,12 +20849,12 @@
       <c r="B14" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="38" t="s">
+      <c r="C14" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="38"/>
+      <c r="D14" s="41"/>
       <c r="E14" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="N14">
         <f t="shared" si="4"/>
@@ -21098,10 +21086,10 @@
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A21" s="41" t="s">
+      <c r="A21" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="41"/>
+      <c r="B21" s="44"/>
       <c r="N21">
         <f t="shared" si="4"/>
         <v>0.13999999999999999</v>
@@ -21175,9 +21163,7 @@
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A24" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="A24" s="1"/>
       <c r="N24">
         <f t="shared" si="4"/>
         <v>0.17</v>
@@ -21200,30 +21186,6 @@
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A25" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H25" s="3" t="s">
-        <v>23</v>
-      </c>
       <c r="N25">
         <f t="shared" si="4"/>
         <v>0.18000000000000002</v>
@@ -21246,36 +21208,6 @@
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A26" s="3">
-        <v>40</v>
-      </c>
-      <c r="B26" s="3">
-        <f t="shared" ref="B26:B66" si="5">A26/GCD(A26,$A$26)</f>
-        <v>1</v>
-      </c>
-      <c r="C26" s="3">
-        <f t="shared" ref="C26:C27" si="6">$A$26/GCD(A26,$A$26)</f>
-        <v>1</v>
-      </c>
-      <c r="D26" s="3">
-        <f>$B$18</f>
-        <v>1.25</v>
-      </c>
-      <c r="E26" s="3">
-        <v>20</v>
-      </c>
-      <c r="F26" s="3">
-        <f>E26/GCD(E26,$E$26)</f>
-        <v>1</v>
-      </c>
-      <c r="G26" s="3">
-        <f>$E$26/GCD(E26,$E$26)</f>
-        <v>1</v>
-      </c>
-      <c r="H26" s="3">
-        <f>$B$18</f>
-        <v>1.25</v>
-      </c>
       <c r="N26">
         <f t="shared" si="4"/>
         <v>0.19000000000000003</v>
@@ -21298,38 +21230,6 @@
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A27" s="3">
-        <f>A26-1</f>
-        <v>39</v>
-      </c>
-      <c r="B27" s="3">
-        <f t="shared" si="5"/>
-        <v>39</v>
-      </c>
-      <c r="C27" s="3">
-        <f t="shared" si="6"/>
-        <v>40</v>
-      </c>
-      <c r="D27" s="3">
-        <f>$D$26*B27/C27</f>
-        <v>1.21875</v>
-      </c>
-      <c r="E27" s="3">
-        <f>E26-1</f>
-        <v>19</v>
-      </c>
-      <c r="F27" s="3">
-        <f>E27/GCD(E27,$E$26)</f>
-        <v>19</v>
-      </c>
-      <c r="G27" s="3">
-        <f>$E$26/GCD(E27,$E$26)</f>
-        <v>20</v>
-      </c>
-      <c r="H27" s="3">
-        <f>$H$26*F27/G27</f>
-        <v>1.1875</v>
-      </c>
       <c r="N27">
         <f t="shared" si="4"/>
         <v>0.20000000000000004</v>
@@ -21352,38 +21252,6 @@
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A28" s="3">
-        <f t="shared" ref="A28:A66" si="7">A27-1</f>
-        <v>38</v>
-      </c>
-      <c r="B28" s="3">
-        <f t="shared" si="5"/>
-        <v>19</v>
-      </c>
-      <c r="C28" s="3">
-        <f t="shared" ref="C28:C66" si="8">$A$26/GCD(A28,$A$26)</f>
-        <v>20</v>
-      </c>
-      <c r="D28" s="3">
-        <f t="shared" ref="D28:D66" si="9">$D$26*B28/C28</f>
-        <v>1.1875</v>
-      </c>
-      <c r="E28" s="3">
-        <f t="shared" ref="E28:E46" si="10">E27-1</f>
-        <v>18</v>
-      </c>
-      <c r="F28" s="3">
-        <f t="shared" ref="F28:F46" si="11">E28/GCD(E28,$E$26)</f>
-        <v>9</v>
-      </c>
-      <c r="G28" s="3">
-        <f t="shared" ref="G28:G46" si="12">$E$26/GCD(E28,$E$26)</f>
-        <v>10</v>
-      </c>
-      <c r="H28" s="3">
-        <f t="shared" ref="H28:H46" si="13">$H$26*F28/G28</f>
-        <v>1.125</v>
-      </c>
       <c r="N28">
         <f t="shared" si="4"/>
         <v>0.21000000000000005</v>
@@ -21406,38 +21274,6 @@
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A29" s="3">
-        <f t="shared" si="7"/>
-        <v>37</v>
-      </c>
-      <c r="B29" s="3">
-        <f t="shared" si="5"/>
-        <v>37</v>
-      </c>
-      <c r="C29" s="3">
-        <f t="shared" si="8"/>
-        <v>40</v>
-      </c>
-      <c r="D29" s="3">
-        <f t="shared" si="9"/>
-        <v>1.15625</v>
-      </c>
-      <c r="E29" s="3">
-        <f t="shared" si="10"/>
-        <v>17</v>
-      </c>
-      <c r="F29" s="3">
-        <f t="shared" si="11"/>
-        <v>17</v>
-      </c>
-      <c r="G29" s="3">
-        <f t="shared" si="12"/>
-        <v>20</v>
-      </c>
-      <c r="H29" s="3">
-        <f t="shared" si="13"/>
-        <v>1.0625</v>
-      </c>
       <c r="N29">
         <f t="shared" si="4"/>
         <v>0.22000000000000006</v>
@@ -21460,38 +21296,6 @@
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A30" s="3">
-        <f t="shared" si="7"/>
-        <v>36</v>
-      </c>
-      <c r="B30" s="3">
-        <f t="shared" si="5"/>
-        <v>9</v>
-      </c>
-      <c r="C30" s="3">
-        <f t="shared" si="8"/>
-        <v>10</v>
-      </c>
-      <c r="D30" s="3">
-        <f t="shared" si="9"/>
-        <v>1.125</v>
-      </c>
-      <c r="E30" s="3">
-        <f t="shared" si="10"/>
-        <v>16</v>
-      </c>
-      <c r="F30" s="3">
-        <f t="shared" si="11"/>
-        <v>4</v>
-      </c>
-      <c r="G30" s="3">
-        <f t="shared" si="12"/>
-        <v>5</v>
-      </c>
-      <c r="H30" s="3">
-        <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
       <c r="N30">
         <f t="shared" si="4"/>
         <v>0.23000000000000007</v>
@@ -21514,38 +21318,6 @@
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A31" s="3">
-        <f t="shared" si="7"/>
-        <v>35</v>
-      </c>
-      <c r="B31" s="3">
-        <f t="shared" si="5"/>
-        <v>7</v>
-      </c>
-      <c r="C31" s="3">
-        <f t="shared" si="8"/>
-        <v>8</v>
-      </c>
-      <c r="D31" s="3">
-        <f t="shared" si="9"/>
-        <v>1.09375</v>
-      </c>
-      <c r="E31" s="3">
-        <f t="shared" si="10"/>
-        <v>15</v>
-      </c>
-      <c r="F31" s="3">
-        <f t="shared" si="11"/>
-        <v>3</v>
-      </c>
-      <c r="G31" s="3">
-        <f t="shared" si="12"/>
-        <v>4</v>
-      </c>
-      <c r="H31" s="3">
-        <f t="shared" si="13"/>
-        <v>0.9375</v>
-      </c>
       <c r="N31">
         <f t="shared" si="4"/>
         <v>0.24000000000000007</v>
@@ -21568,38 +21340,6 @@
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A32" s="3">
-        <f t="shared" si="7"/>
-        <v>34</v>
-      </c>
-      <c r="B32" s="3">
-        <f t="shared" si="5"/>
-        <v>17</v>
-      </c>
-      <c r="C32" s="3">
-        <f t="shared" si="8"/>
-        <v>20</v>
-      </c>
-      <c r="D32" s="3">
-        <f t="shared" si="9"/>
-        <v>1.0625</v>
-      </c>
-      <c r="E32" s="3">
-        <f t="shared" si="10"/>
-        <v>14</v>
-      </c>
-      <c r="F32" s="3">
-        <f t="shared" si="11"/>
-        <v>7</v>
-      </c>
-      <c r="G32" s="3">
-        <f t="shared" si="12"/>
-        <v>10</v>
-      </c>
-      <c r="H32" s="3">
-        <f t="shared" si="13"/>
-        <v>0.875</v>
-      </c>
       <c r="N32">
         <f t="shared" si="4"/>
         <v>0.25000000000000006</v>
@@ -21621,39 +21361,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A33" s="3">
-        <f t="shared" si="7"/>
-        <v>33</v>
-      </c>
-      <c r="B33" s="3">
-        <f t="shared" si="5"/>
-        <v>33</v>
-      </c>
-      <c r="C33" s="3">
-        <f t="shared" si="8"/>
-        <v>40</v>
-      </c>
-      <c r="D33" s="3">
-        <f t="shared" si="9"/>
-        <v>1.03125</v>
-      </c>
-      <c r="E33" s="3">
-        <f t="shared" si="10"/>
-        <v>13</v>
-      </c>
-      <c r="F33" s="3">
-        <f t="shared" si="11"/>
-        <v>13</v>
-      </c>
-      <c r="G33" s="3">
-        <f t="shared" si="12"/>
-        <v>20</v>
-      </c>
-      <c r="H33" s="3">
-        <f t="shared" si="13"/>
-        <v>0.8125</v>
-      </c>
+    <row r="33" spans="14:18" x14ac:dyDescent="0.35">
       <c r="N33">
         <f t="shared" si="4"/>
         <v>0.26000000000000006</v>
@@ -21675,39 +21383,7 @@
         <v>8.3000000000000007</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A34" s="3">
-        <f t="shared" si="7"/>
-        <v>32</v>
-      </c>
-      <c r="B34" s="3">
-        <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-      <c r="C34" s="3">
-        <f t="shared" si="8"/>
-        <v>5</v>
-      </c>
-      <c r="D34" s="3">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="E34" s="3">
-        <f t="shared" si="10"/>
-        <v>12</v>
-      </c>
-      <c r="F34" s="3">
-        <f t="shared" si="11"/>
-        <v>3</v>
-      </c>
-      <c r="G34" s="3">
-        <f t="shared" si="12"/>
-        <v>5</v>
-      </c>
-      <c r="H34" s="3">
-        <f t="shared" si="13"/>
-        <v>0.75</v>
-      </c>
+    <row r="34" spans="14:18" x14ac:dyDescent="0.35">
       <c r="N34">
         <f t="shared" si="4"/>
         <v>0.27000000000000007</v>
@@ -21729,39 +21405,7 @@
         <v>8.6</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A35" s="3">
-        <f t="shared" si="7"/>
-        <v>31</v>
-      </c>
-      <c r="B35" s="3">
-        <f t="shared" si="5"/>
-        <v>31</v>
-      </c>
-      <c r="C35" s="3">
-        <f t="shared" si="8"/>
-        <v>40</v>
-      </c>
-      <c r="D35" s="3">
-        <f t="shared" si="9"/>
-        <v>0.96875</v>
-      </c>
-      <c r="E35" s="3">
-        <f t="shared" si="10"/>
-        <v>11</v>
-      </c>
-      <c r="F35" s="3">
-        <f t="shared" si="11"/>
-        <v>11</v>
-      </c>
-      <c r="G35" s="3">
-        <f t="shared" si="12"/>
-        <v>20</v>
-      </c>
-      <c r="H35" s="3">
-        <f t="shared" si="13"/>
-        <v>0.6875</v>
-      </c>
+    <row r="35" spans="14:18" x14ac:dyDescent="0.35">
       <c r="N35">
         <f t="shared" si="4"/>
         <v>0.28000000000000008</v>
@@ -21783,39 +21427,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A36" s="3">
-        <f t="shared" si="7"/>
-        <v>30</v>
-      </c>
-      <c r="B36" s="3">
-        <f t="shared" si="5"/>
-        <v>3</v>
-      </c>
-      <c r="C36" s="3">
-        <f t="shared" si="8"/>
-        <v>4</v>
-      </c>
-      <c r="D36" s="3">
-        <f t="shared" si="9"/>
-        <v>0.9375</v>
-      </c>
-      <c r="E36" s="3">
-        <f t="shared" si="10"/>
-        <v>10</v>
-      </c>
-      <c r="F36" s="3">
-        <f t="shared" si="11"/>
-        <v>1</v>
-      </c>
-      <c r="G36" s="3">
-        <f t="shared" si="12"/>
-        <v>2</v>
-      </c>
-      <c r="H36" s="3">
-        <f t="shared" si="13"/>
-        <v>0.625</v>
-      </c>
+    <row r="36" spans="14:18" x14ac:dyDescent="0.35">
       <c r="N36">
         <f t="shared" si="4"/>
         <v>0.29000000000000009</v>
@@ -21837,39 +21449,7 @@
         <v>9.3000000000000007</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A37" s="3">
-        <f t="shared" si="7"/>
-        <v>29</v>
-      </c>
-      <c r="B37" s="3">
-        <f t="shared" si="5"/>
-        <v>29</v>
-      </c>
-      <c r="C37" s="3">
-        <f t="shared" si="8"/>
-        <v>40</v>
-      </c>
-      <c r="D37" s="3">
-        <f t="shared" si="9"/>
-        <v>0.90625</v>
-      </c>
-      <c r="E37" s="3">
-        <f t="shared" si="10"/>
-        <v>9</v>
-      </c>
-      <c r="F37" s="3">
-        <f t="shared" si="11"/>
-        <v>9</v>
-      </c>
-      <c r="G37" s="3">
-        <f t="shared" si="12"/>
-        <v>20</v>
-      </c>
-      <c r="H37" s="3">
-        <f t="shared" si="13"/>
-        <v>0.5625</v>
-      </c>
+    <row r="37" spans="14:18" x14ac:dyDescent="0.35">
       <c r="N37">
         <f t="shared" si="4"/>
         <v>0.3000000000000001</v>
@@ -21891,39 +21471,7 @@
         <v>9.6</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A38" s="3">
-        <f t="shared" si="7"/>
-        <v>28</v>
-      </c>
-      <c r="B38" s="3">
-        <f t="shared" si="5"/>
-        <v>7</v>
-      </c>
-      <c r="C38" s="3">
-        <f t="shared" si="8"/>
-        <v>10</v>
-      </c>
-      <c r="D38" s="3">
-        <f t="shared" si="9"/>
-        <v>0.875</v>
-      </c>
-      <c r="E38" s="3">
-        <f t="shared" si="10"/>
-        <v>8</v>
-      </c>
-      <c r="F38" s="3">
-        <f t="shared" si="11"/>
-        <v>2</v>
-      </c>
-      <c r="G38" s="3">
-        <f t="shared" si="12"/>
-        <v>5</v>
-      </c>
-      <c r="H38" s="3">
-        <f t="shared" si="13"/>
-        <v>0.5</v>
-      </c>
+    <row r="38" spans="14:18" x14ac:dyDescent="0.35">
       <c r="N38">
         <f t="shared" si="4"/>
         <v>0.31000000000000011</v>
@@ -21945,39 +21493,7 @@
         <v>9.9</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A39" s="3">
-        <f t="shared" si="7"/>
-        <v>27</v>
-      </c>
-      <c r="B39" s="3">
-        <f t="shared" si="5"/>
-        <v>27</v>
-      </c>
-      <c r="C39" s="3">
-        <f t="shared" si="8"/>
-        <v>40</v>
-      </c>
-      <c r="D39" s="3">
-        <f t="shared" si="9"/>
-        <v>0.84375</v>
-      </c>
-      <c r="E39" s="3">
-        <f t="shared" si="10"/>
-        <v>7</v>
-      </c>
-      <c r="F39" s="3">
-        <f t="shared" si="11"/>
-        <v>7</v>
-      </c>
-      <c r="G39" s="3">
-        <f t="shared" si="12"/>
-        <v>20</v>
-      </c>
-      <c r="H39" s="3">
-        <f t="shared" si="13"/>
-        <v>0.4375</v>
-      </c>
+    <row r="39" spans="14:18" x14ac:dyDescent="0.35">
       <c r="N39">
         <f t="shared" si="4"/>
         <v>0.32000000000000012</v>
@@ -21999,53 +21515,21 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A40" s="3">
-        <f t="shared" si="7"/>
-        <v>26</v>
-      </c>
-      <c r="B40" s="3">
-        <f t="shared" si="5"/>
-        <v>13</v>
-      </c>
-      <c r="C40" s="3">
-        <f t="shared" si="8"/>
-        <v>20</v>
-      </c>
-      <c r="D40" s="3">
-        <f t="shared" si="9"/>
-        <v>0.8125</v>
-      </c>
-      <c r="E40" s="3">
-        <f t="shared" si="10"/>
-        <v>6</v>
-      </c>
-      <c r="F40" s="3">
-        <f t="shared" si="11"/>
-        <v>3</v>
-      </c>
-      <c r="G40" s="3">
-        <f t="shared" si="12"/>
-        <v>10</v>
-      </c>
-      <c r="H40" s="3">
-        <f t="shared" si="13"/>
-        <v>0.375</v>
-      </c>
+    <row r="40" spans="14:18" x14ac:dyDescent="0.35">
       <c r="N40">
         <f t="shared" si="4"/>
         <v>0.33000000000000013</v>
       </c>
       <c r="O40" s="3">
-        <f t="shared" ref="O40:O71" si="14">$O$2*$N40</f>
+        <f t="shared" ref="O40:O71" si="5">$O$2*$N40</f>
         <v>0.66000000000000025</v>
       </c>
       <c r="P40" s="3">
-        <f t="shared" ref="P40:P71" si="15">$O$3*$N40</f>
+        <f t="shared" ref="P40:P71" si="6">$O$3*$N40</f>
         <v>237.60000000000008</v>
       </c>
       <c r="Q40" s="3">
-        <f t="shared" ref="Q40:Q71" si="16">$O$4*$N40</f>
+        <f t="shared" ref="Q40:Q71" si="7">$O$4*$N40</f>
         <v>528.00000000000023</v>
       </c>
       <c r="R40" s="3">
@@ -22053,53 +21537,21 @@
         <v>10.6</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A41" s="3">
-        <f t="shared" si="7"/>
-        <v>25</v>
-      </c>
-      <c r="B41" s="3">
-        <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-      <c r="C41" s="3">
-        <f t="shared" si="8"/>
-        <v>8</v>
-      </c>
-      <c r="D41" s="3">
-        <f t="shared" si="9"/>
-        <v>0.78125</v>
-      </c>
-      <c r="E41" s="3">
-        <f t="shared" si="10"/>
-        <v>5</v>
-      </c>
-      <c r="F41" s="3">
-        <f t="shared" si="11"/>
-        <v>1</v>
-      </c>
-      <c r="G41" s="3">
-        <f t="shared" si="12"/>
-        <v>4</v>
-      </c>
-      <c r="H41" s="3">
-        <f t="shared" si="13"/>
-        <v>0.3125</v>
-      </c>
+    <row r="41" spans="14:18" x14ac:dyDescent="0.35">
       <c r="N41">
         <f t="shared" si="4"/>
         <v>0.34000000000000014</v>
       </c>
       <c r="O41" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="5"/>
         <v>0.68000000000000027</v>
       </c>
       <c r="P41" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="6"/>
         <v>244.8000000000001</v>
       </c>
       <c r="Q41" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="7"/>
         <v>544.00000000000023</v>
       </c>
       <c r="R41" s="3">
@@ -22107,53 +21559,21 @@
         <v>10.9</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A42" s="3">
-        <f t="shared" si="7"/>
-        <v>24</v>
-      </c>
-      <c r="B42" s="3">
-        <f t="shared" si="5"/>
-        <v>3</v>
-      </c>
-      <c r="C42" s="3">
-        <f t="shared" si="8"/>
-        <v>5</v>
-      </c>
-      <c r="D42" s="3">
-        <f t="shared" si="9"/>
-        <v>0.75</v>
-      </c>
-      <c r="E42" s="3">
-        <f t="shared" si="10"/>
-        <v>4</v>
-      </c>
-      <c r="F42" s="3">
-        <f t="shared" si="11"/>
-        <v>1</v>
-      </c>
-      <c r="G42" s="3">
-        <f t="shared" si="12"/>
-        <v>5</v>
-      </c>
-      <c r="H42" s="3">
-        <f t="shared" si="13"/>
-        <v>0.25</v>
-      </c>
+    <row r="42" spans="14:18" x14ac:dyDescent="0.35">
       <c r="N42">
         <f t="shared" si="4"/>
         <v>0.35000000000000014</v>
       </c>
       <c r="O42" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="5"/>
         <v>0.70000000000000029</v>
       </c>
       <c r="P42" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="6"/>
         <v>252.00000000000011</v>
       </c>
       <c r="Q42" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="7"/>
         <v>560.00000000000023</v>
       </c>
       <c r="R42" s="3">
@@ -22161,53 +21581,21 @@
         <v>11.2</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A43" s="3">
-        <f t="shared" si="7"/>
-        <v>23</v>
-      </c>
-      <c r="B43" s="3">
-        <f t="shared" si="5"/>
-        <v>23</v>
-      </c>
-      <c r="C43" s="3">
-        <f t="shared" si="8"/>
-        <v>40</v>
-      </c>
-      <c r="D43" s="3">
-        <f t="shared" si="9"/>
-        <v>0.71875</v>
-      </c>
-      <c r="E43" s="3">
-        <f t="shared" si="10"/>
-        <v>3</v>
-      </c>
-      <c r="F43" s="3">
-        <f t="shared" si="11"/>
-        <v>3</v>
-      </c>
-      <c r="G43" s="3">
-        <f t="shared" si="12"/>
-        <v>20</v>
-      </c>
-      <c r="H43" s="3">
-        <f t="shared" si="13"/>
-        <v>0.1875</v>
-      </c>
+    <row r="43" spans="14:18" x14ac:dyDescent="0.35">
       <c r="N43">
         <f t="shared" si="4"/>
         <v>0.36000000000000015</v>
       </c>
       <c r="O43" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="5"/>
         <v>0.72000000000000031</v>
       </c>
       <c r="P43" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="6"/>
         <v>259.2000000000001</v>
       </c>
       <c r="Q43" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="7"/>
         <v>576.00000000000023</v>
       </c>
       <c r="R43" s="3">
@@ -22215,53 +21603,21 @@
         <v>11.5</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A44" s="3">
-        <f t="shared" si="7"/>
-        <v>22</v>
-      </c>
-      <c r="B44" s="3">
-        <f t="shared" si="5"/>
-        <v>11</v>
-      </c>
-      <c r="C44" s="3">
-        <f t="shared" si="8"/>
-        <v>20</v>
-      </c>
-      <c r="D44" s="3">
-        <f t="shared" si="9"/>
-        <v>0.6875</v>
-      </c>
-      <c r="E44" s="3">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-      <c r="F44" s="3">
-        <f t="shared" si="11"/>
-        <v>1</v>
-      </c>
-      <c r="G44" s="3">
-        <f t="shared" si="12"/>
-        <v>10</v>
-      </c>
-      <c r="H44" s="3">
-        <f t="shared" si="13"/>
-        <v>0.125</v>
-      </c>
+    <row r="44" spans="14:18" x14ac:dyDescent="0.35">
       <c r="N44">
         <f t="shared" si="4"/>
         <v>0.37000000000000016</v>
       </c>
       <c r="O44" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="5"/>
         <v>0.74000000000000032</v>
       </c>
       <c r="P44" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="6"/>
         <v>266.40000000000009</v>
       </c>
       <c r="Q44" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="7"/>
         <v>592.00000000000023</v>
       </c>
       <c r="R44" s="3">
@@ -22269,53 +21625,21 @@
         <v>11.8</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A45" s="3">
-        <f t="shared" si="7"/>
-        <v>21</v>
-      </c>
-      <c r="B45" s="3">
-        <f t="shared" si="5"/>
-        <v>21</v>
-      </c>
-      <c r="C45" s="3">
-        <f t="shared" si="8"/>
-        <v>40</v>
-      </c>
-      <c r="D45" s="3">
-        <f t="shared" si="9"/>
-        <v>0.65625</v>
-      </c>
-      <c r="E45" s="3">
-        <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="F45" s="3">
-        <f t="shared" si="11"/>
-        <v>1</v>
-      </c>
-      <c r="G45" s="3">
-        <f t="shared" si="12"/>
-        <v>20</v>
-      </c>
-      <c r="H45" s="3">
-        <f t="shared" si="13"/>
-        <v>6.25E-2</v>
-      </c>
+    <row r="45" spans="14:18" x14ac:dyDescent="0.35">
       <c r="N45">
         <f t="shared" si="4"/>
         <v>0.38000000000000017</v>
       </c>
       <c r="O45" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="5"/>
         <v>0.76000000000000034</v>
       </c>
       <c r="P45" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="6"/>
         <v>273.60000000000014</v>
       </c>
       <c r="Q45" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="7"/>
         <v>608.00000000000023</v>
       </c>
       <c r="R45" s="3">
@@ -22323,53 +21647,21 @@
         <v>12.2</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A46" s="3">
-        <f t="shared" si="7"/>
-        <v>20</v>
-      </c>
-      <c r="B46" s="3">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="C46" s="3">
-        <f t="shared" si="8"/>
-        <v>2</v>
-      </c>
-      <c r="D46" s="3">
-        <f t="shared" si="9"/>
-        <v>0.625</v>
-      </c>
-      <c r="E46" s="3">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="F46" s="3">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="G46" s="3">
-        <f t="shared" si="12"/>
-        <v>1</v>
-      </c>
-      <c r="H46" s="3">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
+    <row r="46" spans="14:18" x14ac:dyDescent="0.35">
       <c r="N46">
         <f t="shared" si="4"/>
         <v>0.39000000000000018</v>
       </c>
       <c r="O46" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="5"/>
         <v>0.78000000000000036</v>
       </c>
       <c r="P46" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="6"/>
         <v>280.80000000000013</v>
       </c>
       <c r="Q46" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="7"/>
         <v>624.00000000000034</v>
       </c>
       <c r="R46" s="3">
@@ -22377,37 +21669,21 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A47" s="3">
-        <f t="shared" si="7"/>
-        <v>19</v>
-      </c>
-      <c r="B47" s="3">
-        <f t="shared" si="5"/>
-        <v>19</v>
-      </c>
-      <c r="C47" s="3">
-        <f t="shared" si="8"/>
-        <v>40</v>
-      </c>
-      <c r="D47" s="3">
-        <f t="shared" si="9"/>
-        <v>0.59375</v>
-      </c>
+    <row r="47" spans="14:18" x14ac:dyDescent="0.35">
       <c r="N47">
         <f t="shared" si="4"/>
         <v>0.40000000000000019</v>
       </c>
       <c r="O47" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="5"/>
         <v>0.80000000000000038</v>
       </c>
       <c r="P47" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="6"/>
         <v>288.00000000000011</v>
       </c>
       <c r="Q47" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="7"/>
         <v>640.00000000000034</v>
       </c>
       <c r="R47" s="3">
@@ -22415,37 +21691,21 @@
         <v>12.8</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A48" s="3">
-        <f t="shared" si="7"/>
-        <v>18</v>
-      </c>
-      <c r="B48" s="3">
-        <f t="shared" si="5"/>
-        <v>9</v>
-      </c>
-      <c r="C48" s="3">
-        <f t="shared" si="8"/>
-        <v>20</v>
-      </c>
-      <c r="D48" s="3">
-        <f t="shared" si="9"/>
-        <v>0.5625</v>
-      </c>
+    <row r="48" spans="14:18" x14ac:dyDescent="0.35">
       <c r="N48">
         <f t="shared" si="4"/>
         <v>0.4100000000000002</v>
       </c>
       <c r="O48" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="5"/>
         <v>0.8200000000000004</v>
       </c>
       <c r="P48" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="6"/>
         <v>295.20000000000016</v>
       </c>
       <c r="Q48" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="7"/>
         <v>656.00000000000034</v>
       </c>
       <c r="R48" s="3">
@@ -22453,37 +21713,21 @@
         <v>13.1</v>
       </c>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A49" s="3">
-        <f t="shared" si="7"/>
-        <v>17</v>
-      </c>
-      <c r="B49" s="3">
-        <f t="shared" si="5"/>
-        <v>17</v>
-      </c>
-      <c r="C49" s="3">
-        <f t="shared" si="8"/>
-        <v>40</v>
-      </c>
-      <c r="D49" s="3">
-        <f t="shared" si="9"/>
-        <v>0.53125</v>
-      </c>
+    <row r="49" spans="14:18" x14ac:dyDescent="0.35">
       <c r="N49">
         <f t="shared" si="4"/>
         <v>0.42000000000000021</v>
       </c>
       <c r="O49" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="5"/>
         <v>0.84000000000000041</v>
       </c>
       <c r="P49" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="6"/>
         <v>302.40000000000015</v>
       </c>
       <c r="Q49" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="7"/>
         <v>672.00000000000034</v>
       </c>
       <c r="R49" s="3">
@@ -22491,37 +21735,21 @@
         <v>13.4</v>
       </c>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A50" s="3">
-        <f t="shared" si="7"/>
-        <v>16</v>
-      </c>
-      <c r="B50" s="3">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="C50" s="3">
-        <f t="shared" si="8"/>
-        <v>5</v>
-      </c>
-      <c r="D50" s="3">
-        <f t="shared" si="9"/>
-        <v>0.5</v>
-      </c>
+    <row r="50" spans="14:18" x14ac:dyDescent="0.35">
       <c r="N50">
         <f t="shared" si="4"/>
         <v>0.43000000000000022</v>
       </c>
       <c r="O50" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="5"/>
         <v>0.86000000000000043</v>
       </c>
       <c r="P50" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="6"/>
         <v>309.60000000000014</v>
       </c>
       <c r="Q50" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="7"/>
         <v>688.00000000000034</v>
       </c>
       <c r="R50" s="3">
@@ -22529,37 +21757,21 @@
         <v>13.8</v>
       </c>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A51" s="3">
-        <f t="shared" si="7"/>
-        <v>15</v>
-      </c>
-      <c r="B51" s="3">
-        <f t="shared" si="5"/>
-        <v>3</v>
-      </c>
-      <c r="C51" s="3">
-        <f t="shared" si="8"/>
-        <v>8</v>
-      </c>
-      <c r="D51" s="3">
-        <f t="shared" si="9"/>
-        <v>0.46875</v>
-      </c>
+    <row r="51" spans="14:18" x14ac:dyDescent="0.35">
       <c r="N51">
         <f t="shared" si="4"/>
         <v>0.44000000000000022</v>
       </c>
       <c r="O51" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="5"/>
         <v>0.88000000000000045</v>
       </c>
       <c r="P51" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="6"/>
         <v>316.80000000000018</v>
       </c>
       <c r="Q51" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="7"/>
         <v>704.00000000000034</v>
       </c>
       <c r="R51" s="3">
@@ -22567,37 +21779,21 @@
         <v>14.1</v>
       </c>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A52" s="3">
-        <f t="shared" si="7"/>
-        <v>14</v>
-      </c>
-      <c r="B52" s="3">
-        <f t="shared" si="5"/>
-        <v>7</v>
-      </c>
-      <c r="C52" s="3">
-        <f t="shared" si="8"/>
-        <v>20</v>
-      </c>
-      <c r="D52" s="3">
-        <f t="shared" si="9"/>
-        <v>0.4375</v>
-      </c>
+    <row r="52" spans="14:18" x14ac:dyDescent="0.35">
       <c r="N52">
         <f t="shared" si="4"/>
         <v>0.45000000000000023</v>
       </c>
       <c r="O52" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="5"/>
         <v>0.90000000000000047</v>
       </c>
       <c r="P52" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="6"/>
         <v>324.00000000000017</v>
       </c>
       <c r="Q52" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="7"/>
         <v>720.00000000000034</v>
       </c>
       <c r="R52" s="3">
@@ -22605,37 +21801,21 @@
         <v>14.4</v>
       </c>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A53" s="3">
-        <f t="shared" si="7"/>
-        <v>13</v>
-      </c>
-      <c r="B53" s="3">
-        <f t="shared" si="5"/>
-        <v>13</v>
-      </c>
-      <c r="C53" s="3">
-        <f t="shared" si="8"/>
-        <v>40</v>
-      </c>
-      <c r="D53" s="3">
-        <f t="shared" si="9"/>
-        <v>0.40625</v>
-      </c>
+    <row r="53" spans="14:18" x14ac:dyDescent="0.35">
       <c r="N53">
         <f t="shared" si="4"/>
         <v>0.46000000000000024</v>
       </c>
       <c r="O53" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="5"/>
         <v>0.92000000000000048</v>
       </c>
       <c r="P53" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="6"/>
         <v>331.20000000000016</v>
       </c>
       <c r="Q53" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="7"/>
         <v>736.00000000000034</v>
       </c>
       <c r="R53" s="3">
@@ -22643,37 +21823,21 @@
         <v>14.7</v>
       </c>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A54" s="3">
-        <f t="shared" si="7"/>
-        <v>12</v>
-      </c>
-      <c r="B54" s="3">
-        <f t="shared" si="5"/>
-        <v>3</v>
-      </c>
-      <c r="C54" s="3">
-        <f t="shared" si="8"/>
-        <v>10</v>
-      </c>
-      <c r="D54" s="3">
-        <f t="shared" si="9"/>
-        <v>0.375</v>
-      </c>
+    <row r="54" spans="14:18" x14ac:dyDescent="0.35">
       <c r="N54">
         <f t="shared" si="4"/>
         <v>0.47000000000000025</v>
       </c>
       <c r="O54" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="5"/>
         <v>0.9400000000000005</v>
       </c>
       <c r="P54" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="6"/>
         <v>338.4000000000002</v>
       </c>
       <c r="Q54" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="7"/>
         <v>752.00000000000045</v>
       </c>
       <c r="R54" s="3">
@@ -22681,37 +21845,21 @@
         <v>15</v>
       </c>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A55" s="3">
-        <f t="shared" si="7"/>
-        <v>11</v>
-      </c>
-      <c r="B55" s="3">
-        <f t="shared" si="5"/>
-        <v>11</v>
-      </c>
-      <c r="C55" s="3">
-        <f t="shared" si="8"/>
-        <v>40</v>
-      </c>
-      <c r="D55" s="3">
-        <f t="shared" si="9"/>
-        <v>0.34375</v>
-      </c>
+    <row r="55" spans="14:18" x14ac:dyDescent="0.35">
       <c r="N55">
         <f t="shared" si="4"/>
         <v>0.48000000000000026</v>
       </c>
       <c r="O55" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="5"/>
         <v>0.96000000000000052</v>
       </c>
       <c r="P55" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="6"/>
         <v>345.60000000000019</v>
       </c>
       <c r="Q55" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="7"/>
         <v>768.00000000000045</v>
       </c>
       <c r="R55" s="3">
@@ -22719,37 +21867,21 @@
         <v>15.4</v>
       </c>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A56" s="3">
-        <f t="shared" si="7"/>
-        <v>10</v>
-      </c>
-      <c r="B56" s="3">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="C56" s="3">
-        <f t="shared" si="8"/>
-        <v>4</v>
-      </c>
-      <c r="D56" s="3">
-        <f t="shared" si="9"/>
-        <v>0.3125</v>
-      </c>
+    <row r="56" spans="14:18" x14ac:dyDescent="0.35">
       <c r="N56">
         <f t="shared" si="4"/>
         <v>0.49000000000000027</v>
       </c>
       <c r="O56" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="5"/>
         <v>0.98000000000000054</v>
       </c>
       <c r="P56" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="6"/>
         <v>352.80000000000018</v>
       </c>
       <c r="Q56" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="7"/>
         <v>784.00000000000045</v>
       </c>
       <c r="R56" s="3">
@@ -22757,37 +21889,21 @@
         <v>15.7</v>
       </c>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A57" s="3">
-        <f t="shared" si="7"/>
-        <v>9</v>
-      </c>
-      <c r="B57" s="3">
-        <f t="shared" si="5"/>
-        <v>9</v>
-      </c>
-      <c r="C57" s="3">
-        <f t="shared" si="8"/>
-        <v>40</v>
-      </c>
-      <c r="D57" s="3">
-        <f t="shared" si="9"/>
-        <v>0.28125</v>
-      </c>
+    <row r="57" spans="14:18" x14ac:dyDescent="0.35">
       <c r="N57">
         <f t="shared" si="4"/>
         <v>0.50000000000000022</v>
       </c>
       <c r="O57" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="5"/>
         <v>1.0000000000000004</v>
       </c>
       <c r="P57" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="6"/>
         <v>360.00000000000017</v>
       </c>
       <c r="Q57" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="7"/>
         <v>800.00000000000034</v>
       </c>
       <c r="R57" s="3">
@@ -22795,37 +21911,21 @@
         <v>16</v>
       </c>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A58" s="3">
-        <f t="shared" si="7"/>
-        <v>8</v>
-      </c>
-      <c r="B58" s="3">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="C58" s="3">
-        <f t="shared" si="8"/>
-        <v>5</v>
-      </c>
-      <c r="D58" s="3">
-        <f t="shared" si="9"/>
-        <v>0.25</v>
-      </c>
+    <row r="58" spans="14:18" x14ac:dyDescent="0.35">
       <c r="N58">
         <f t="shared" si="4"/>
         <v>0.51000000000000023</v>
       </c>
       <c r="O58" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="5"/>
         <v>1.0200000000000005</v>
       </c>
       <c r="P58" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="6"/>
         <v>367.20000000000016</v>
       </c>
       <c r="Q58" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="7"/>
         <v>816.00000000000034</v>
       </c>
       <c r="R58" s="3">
@@ -22833,37 +21933,21 @@
         <v>16.3</v>
       </c>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A59" s="3">
-        <f t="shared" si="7"/>
-        <v>7</v>
-      </c>
-      <c r="B59" s="3">
-        <f t="shared" si="5"/>
-        <v>7</v>
-      </c>
-      <c r="C59" s="3">
-        <f t="shared" si="8"/>
-        <v>40</v>
-      </c>
-      <c r="D59" s="3">
-        <f t="shared" si="9"/>
-        <v>0.21875</v>
-      </c>
+    <row r="59" spans="14:18" x14ac:dyDescent="0.35">
       <c r="N59">
         <f t="shared" si="4"/>
         <v>0.52000000000000024</v>
       </c>
       <c r="O59" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="5"/>
         <v>1.0400000000000005</v>
       </c>
       <c r="P59" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="6"/>
         <v>374.40000000000015</v>
       </c>
       <c r="Q59" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="7"/>
         <v>832.00000000000034</v>
       </c>
       <c r="R59" s="3">
@@ -22871,37 +21955,21 @@
         <v>16.600000000000001</v>
       </c>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A60" s="3">
-        <f t="shared" si="7"/>
-        <v>6</v>
-      </c>
-      <c r="B60" s="3">
-        <f t="shared" si="5"/>
-        <v>3</v>
-      </c>
-      <c r="C60" s="3">
-        <f t="shared" si="8"/>
-        <v>20</v>
-      </c>
-      <c r="D60" s="3">
-        <f t="shared" si="9"/>
-        <v>0.1875</v>
-      </c>
+    <row r="60" spans="14:18" x14ac:dyDescent="0.35">
       <c r="N60">
         <f t="shared" si="4"/>
         <v>0.53000000000000025</v>
       </c>
       <c r="O60" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="5"/>
         <v>1.0600000000000005</v>
       </c>
       <c r="P60" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="6"/>
         <v>381.60000000000019</v>
       </c>
       <c r="Q60" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="7"/>
         <v>848.00000000000045</v>
       </c>
       <c r="R60" s="3">
@@ -22909,37 +21977,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A61" s="3">
-        <f t="shared" si="7"/>
-        <v>5</v>
-      </c>
-      <c r="B61" s="3">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="C61" s="3">
-        <f t="shared" si="8"/>
-        <v>8</v>
-      </c>
-      <c r="D61" s="3">
-        <f t="shared" si="9"/>
-        <v>0.15625</v>
-      </c>
+    <row r="61" spans="14:18" x14ac:dyDescent="0.35">
       <c r="N61">
         <f t="shared" si="4"/>
         <v>0.54000000000000026</v>
       </c>
       <c r="O61" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="5"/>
         <v>1.0800000000000005</v>
       </c>
       <c r="P61" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="6"/>
         <v>388.80000000000018</v>
       </c>
       <c r="Q61" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="7"/>
         <v>864.00000000000045</v>
       </c>
       <c r="R61" s="3">
@@ -22947,37 +21999,21 @@
         <v>17.3</v>
       </c>
     </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A62" s="3">
-        <f t="shared" si="7"/>
-        <v>4</v>
-      </c>
-      <c r="B62" s="3">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="C62" s="3">
-        <f t="shared" si="8"/>
-        <v>10</v>
-      </c>
-      <c r="D62" s="3">
-        <f t="shared" si="9"/>
-        <v>0.125</v>
-      </c>
+    <row r="62" spans="14:18" x14ac:dyDescent="0.35">
       <c r="N62">
         <f t="shared" si="4"/>
         <v>0.55000000000000027</v>
       </c>
       <c r="O62" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="5"/>
         <v>1.1000000000000005</v>
       </c>
       <c r="P62" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="6"/>
         <v>396.00000000000017</v>
       </c>
       <c r="Q62" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="7"/>
         <v>880.00000000000045</v>
       </c>
       <c r="R62" s="3">
@@ -22985,37 +22021,21 @@
         <v>17.600000000000001</v>
       </c>
     </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A63" s="3">
-        <f t="shared" si="7"/>
-        <v>3</v>
-      </c>
-      <c r="B63" s="3">
-        <f t="shared" si="5"/>
-        <v>3</v>
-      </c>
-      <c r="C63" s="3">
-        <f t="shared" si="8"/>
-        <v>40</v>
-      </c>
-      <c r="D63" s="3">
-        <f t="shared" si="9"/>
-        <v>9.375E-2</v>
-      </c>
+    <row r="63" spans="14:18" x14ac:dyDescent="0.35">
       <c r="N63">
         <f t="shared" si="4"/>
         <v>0.56000000000000028</v>
       </c>
       <c r="O63" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="5"/>
         <v>1.1200000000000006</v>
       </c>
       <c r="P63" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="6"/>
         <v>403.20000000000022</v>
       </c>
       <c r="Q63" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="7"/>
         <v>896.00000000000045</v>
       </c>
       <c r="R63" s="3">
@@ -23023,37 +22043,21 @@
         <v>17.899999999999999</v>
       </c>
     </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A64" s="3">
-        <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-      <c r="B64" s="3">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="C64" s="3">
-        <f t="shared" si="8"/>
-        <v>20</v>
-      </c>
-      <c r="D64" s="3">
-        <f t="shared" si="9"/>
-        <v>6.25E-2</v>
-      </c>
+    <row r="64" spans="14:18" x14ac:dyDescent="0.35">
       <c r="N64">
         <f t="shared" si="4"/>
         <v>0.57000000000000028</v>
       </c>
       <c r="O64" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="5"/>
         <v>1.1400000000000006</v>
       </c>
       <c r="P64" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="6"/>
         <v>410.4000000000002</v>
       </c>
       <c r="Q64" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="7"/>
         <v>912.00000000000045</v>
       </c>
       <c r="R64" s="3">
@@ -23061,37 +22065,21 @@
         <v>18.2</v>
       </c>
     </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A65" s="3">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="B65" s="3">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="C65" s="3">
-        <f t="shared" si="8"/>
-        <v>40</v>
-      </c>
-      <c r="D65" s="3">
-        <f t="shared" si="9"/>
-        <v>3.125E-2</v>
-      </c>
+    <row r="65" spans="14:18" x14ac:dyDescent="0.35">
       <c r="N65">
         <f t="shared" si="4"/>
         <v>0.58000000000000029</v>
       </c>
       <c r="O65" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="5"/>
         <v>1.1600000000000006</v>
       </c>
       <c r="P65" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="6"/>
         <v>417.60000000000019</v>
       </c>
       <c r="Q65" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="7"/>
         <v>928.00000000000045</v>
       </c>
       <c r="R65" s="3">
@@ -23099,37 +22087,21 @@
         <v>18.600000000000001</v>
       </c>
     </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A66" s="3">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="B66" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="C66" s="3">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="D66" s="3">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
+    <row r="66" spans="14:18" x14ac:dyDescent="0.35">
       <c r="N66">
         <f t="shared" si="4"/>
         <v>0.5900000000000003</v>
       </c>
       <c r="O66" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="5"/>
         <v>1.1800000000000006</v>
       </c>
       <c r="P66" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="6"/>
         <v>424.80000000000024</v>
       </c>
       <c r="Q66" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="7"/>
         <v>944.00000000000045</v>
       </c>
       <c r="R66" s="3">
@@ -23137,21 +22109,21 @@
         <v>18.899999999999999</v>
       </c>
     </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="67" spans="14:18" x14ac:dyDescent="0.35">
       <c r="N67">
         <f t="shared" si="4"/>
         <v>0.60000000000000031</v>
       </c>
       <c r="O67" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="5"/>
         <v>1.2000000000000006</v>
       </c>
       <c r="P67" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="6"/>
         <v>432.00000000000023</v>
       </c>
       <c r="Q67" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="7"/>
         <v>960.00000000000045</v>
       </c>
       <c r="R67" s="3">
@@ -23159,21 +22131,21 @@
         <v>19.2</v>
       </c>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="68" spans="14:18" x14ac:dyDescent="0.35">
       <c r="N68">
         <f t="shared" si="4"/>
         <v>0.61000000000000032</v>
       </c>
       <c r="O68" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="5"/>
         <v>1.2200000000000006</v>
       </c>
       <c r="P68" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="6"/>
         <v>439.20000000000022</v>
       </c>
       <c r="Q68" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="7"/>
         <v>976.00000000000045</v>
       </c>
       <c r="R68" s="3">
@@ -23181,21 +22153,21 @@
         <v>19.5</v>
       </c>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="69" spans="14:18" x14ac:dyDescent="0.35">
       <c r="N69">
         <f t="shared" si="4"/>
         <v>0.62000000000000033</v>
       </c>
       <c r="O69" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="5"/>
         <v>1.2400000000000007</v>
       </c>
       <c r="P69" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="6"/>
         <v>446.40000000000026</v>
       </c>
       <c r="Q69" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="7"/>
         <v>992.00000000000057</v>
       </c>
       <c r="R69" s="3">
@@ -23203,21 +22175,21 @@
         <v>19.8</v>
       </c>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="70" spans="14:18" x14ac:dyDescent="0.35">
       <c r="N70">
         <f t="shared" si="4"/>
         <v>0.63000000000000034</v>
       </c>
       <c r="O70" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="5"/>
         <v>1.2600000000000007</v>
       </c>
       <c r="P70" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="6"/>
         <v>453.60000000000025</v>
       </c>
       <c r="Q70" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="7"/>
         <v>1008.0000000000006</v>
       </c>
       <c r="R70" s="3">
@@ -23225,21 +22197,21 @@
         <v>20.2</v>
       </c>
     </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="71" spans="14:18" x14ac:dyDescent="0.35">
       <c r="N71">
         <f t="shared" si="4"/>
         <v>0.64000000000000035</v>
       </c>
       <c r="O71" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="5"/>
         <v>1.2800000000000007</v>
       </c>
       <c r="P71" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="6"/>
         <v>460.80000000000024</v>
       </c>
       <c r="Q71" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="7"/>
         <v>1024.0000000000005</v>
       </c>
       <c r="R71" s="3">
@@ -23247,21 +22219,21 @@
         <v>20.5</v>
       </c>
     </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="72" spans="14:18" x14ac:dyDescent="0.35">
       <c r="N72">
         <f t="shared" si="4"/>
         <v>0.65000000000000036</v>
       </c>
       <c r="O72" s="3">
-        <f t="shared" ref="O72:O107" si="17">$O$2*$N72</f>
+        <f t="shared" ref="O72:O107" si="8">$O$2*$N72</f>
         <v>1.3000000000000007</v>
       </c>
       <c r="P72" s="3">
-        <f t="shared" ref="P72:P107" si="18">$O$3*$N72</f>
+        <f t="shared" ref="P72:P107" si="9">$O$3*$N72</f>
         <v>468.00000000000023</v>
       </c>
       <c r="Q72" s="3">
-        <f t="shared" ref="Q72:Q107" si="19">$O$4*$N72</f>
+        <f t="shared" ref="Q72:Q107" si="10">$O$4*$N72</f>
         <v>1040.0000000000005</v>
       </c>
       <c r="R72" s="3">
@@ -23269,773 +22241,773 @@
         <v>20.8</v>
       </c>
     </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="73" spans="14:18" x14ac:dyDescent="0.35">
       <c r="N73">
         <f t="shared" si="4"/>
         <v>0.66000000000000036</v>
       </c>
       <c r="O73" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="8"/>
         <v>1.3200000000000007</v>
       </c>
       <c r="P73" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="9"/>
         <v>475.20000000000027</v>
       </c>
       <c r="Q73" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="10"/>
         <v>1056.0000000000007</v>
       </c>
       <c r="R73" s="3">
-        <f t="shared" ref="R73:R107" si="20">ROUND( (($Q$5/($E$5) / 1.25)*Q73), 1)</f>
+        <f t="shared" ref="R73:R107" si="11">ROUND( (($Q$5/($E$5) / 1.25)*Q73), 1)</f>
         <v>21.1</v>
       </c>
     </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="74" spans="14:18" x14ac:dyDescent="0.35">
       <c r="N74">
-        <f t="shared" ref="N74:N107" si="21">N73+0.01</f>
+        <f t="shared" ref="N74:N107" si="12">N73+0.01</f>
         <v>0.67000000000000037</v>
       </c>
       <c r="O74" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="8"/>
         <v>1.3400000000000007</v>
       </c>
       <c r="P74" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="9"/>
         <v>482.40000000000026</v>
       </c>
       <c r="Q74" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="10"/>
         <v>1072.0000000000007</v>
       </c>
       <c r="R74" s="3">
-        <f t="shared" si="20"/>
+        <f t="shared" si="11"/>
         <v>21.4</v>
       </c>
     </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="75" spans="14:18" x14ac:dyDescent="0.35">
       <c r="N75">
-        <f t="shared" si="21"/>
+        <f t="shared" si="12"/>
         <v>0.68000000000000038</v>
       </c>
       <c r="O75" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="8"/>
         <v>1.3600000000000008</v>
       </c>
       <c r="P75" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="9"/>
         <v>489.60000000000025</v>
       </c>
       <c r="Q75" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="10"/>
         <v>1088.0000000000007</v>
       </c>
       <c r="R75" s="3">
-        <f t="shared" si="20"/>
+        <f t="shared" si="11"/>
         <v>21.8</v>
       </c>
     </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="76" spans="14:18" x14ac:dyDescent="0.35">
       <c r="N76">
-        <f t="shared" si="21"/>
+        <f t="shared" si="12"/>
         <v>0.69000000000000039</v>
       </c>
       <c r="O76" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="8"/>
         <v>1.3800000000000008</v>
       </c>
       <c r="P76" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="9"/>
         <v>496.8000000000003</v>
       </c>
       <c r="Q76" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="10"/>
         <v>1104.0000000000007</v>
       </c>
       <c r="R76" s="3">
-        <f t="shared" si="20"/>
+        <f t="shared" si="11"/>
         <v>22.1</v>
       </c>
     </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="77" spans="14:18" x14ac:dyDescent="0.35">
       <c r="N77">
-        <f t="shared" si="21"/>
+        <f t="shared" si="12"/>
         <v>0.7000000000000004</v>
       </c>
       <c r="O77" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="8"/>
         <v>1.4000000000000008</v>
       </c>
       <c r="P77" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="9"/>
         <v>504.00000000000028</v>
       </c>
       <c r="Q77" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="10"/>
         <v>1120.0000000000007</v>
       </c>
       <c r="R77" s="3">
-        <f t="shared" si="20"/>
+        <f t="shared" si="11"/>
         <v>22.4</v>
       </c>
     </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="78" spans="14:18" x14ac:dyDescent="0.35">
       <c r="N78">
-        <f t="shared" si="21"/>
+        <f t="shared" si="12"/>
         <v>0.71000000000000041</v>
       </c>
       <c r="O78" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="8"/>
         <v>1.4200000000000008</v>
       </c>
       <c r="P78" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="9"/>
         <v>511.20000000000027</v>
       </c>
       <c r="Q78" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="10"/>
         <v>1136.0000000000007</v>
       </c>
       <c r="R78" s="3">
-        <f t="shared" si="20"/>
+        <f t="shared" si="11"/>
         <v>22.7</v>
       </c>
     </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="79" spans="14:18" x14ac:dyDescent="0.35">
       <c r="N79">
-        <f t="shared" si="21"/>
+        <f t="shared" si="12"/>
         <v>0.72000000000000042</v>
       </c>
       <c r="O79" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="8"/>
         <v>1.4400000000000008</v>
       </c>
       <c r="P79" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="9"/>
         <v>518.40000000000032</v>
       </c>
       <c r="Q79" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="10"/>
         <v>1152.0000000000007</v>
       </c>
       <c r="R79" s="3">
-        <f t="shared" si="20"/>
+        <f t="shared" si="11"/>
         <v>23</v>
       </c>
     </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="80" spans="14:18" x14ac:dyDescent="0.35">
       <c r="N80">
-        <f t="shared" si="21"/>
+        <f t="shared" si="12"/>
         <v>0.73000000000000043</v>
       </c>
       <c r="O80" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="8"/>
         <v>1.4600000000000009</v>
       </c>
       <c r="P80" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="9"/>
         <v>525.60000000000036</v>
       </c>
       <c r="Q80" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="10"/>
         <v>1168.0000000000007</v>
       </c>
       <c r="R80" s="3">
-        <f t="shared" si="20"/>
+        <f t="shared" si="11"/>
         <v>23.4</v>
       </c>
     </row>
     <row r="81" spans="14:18" x14ac:dyDescent="0.35">
       <c r="N81">
-        <f t="shared" si="21"/>
+        <f t="shared" si="12"/>
         <v>0.74000000000000044</v>
       </c>
       <c r="O81" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="8"/>
         <v>1.4800000000000009</v>
       </c>
       <c r="P81" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="9"/>
         <v>532.8000000000003</v>
       </c>
       <c r="Q81" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="10"/>
         <v>1184.0000000000007</v>
       </c>
       <c r="R81" s="3">
-        <f t="shared" si="20"/>
+        <f t="shared" si="11"/>
         <v>23.7</v>
       </c>
     </row>
     <row r="82" spans="14:18" x14ac:dyDescent="0.35">
       <c r="N82">
-        <f t="shared" si="21"/>
+        <f t="shared" si="12"/>
         <v>0.75000000000000044</v>
       </c>
       <c r="O82" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="8"/>
         <v>1.5000000000000009</v>
       </c>
       <c r="P82" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="9"/>
         <v>540.00000000000034</v>
       </c>
       <c r="Q82" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="10"/>
         <v>1200.0000000000007</v>
       </c>
       <c r="R82" s="3">
-        <f t="shared" si="20"/>
+        <f t="shared" si="11"/>
         <v>24</v>
       </c>
     </row>
     <row r="83" spans="14:18" x14ac:dyDescent="0.35">
       <c r="N83">
-        <f t="shared" si="21"/>
+        <f t="shared" si="12"/>
         <v>0.76000000000000045</v>
       </c>
       <c r="O83" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="8"/>
         <v>1.5200000000000009</v>
       </c>
       <c r="P83" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="9"/>
         <v>547.20000000000027</v>
       </c>
       <c r="Q83" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="10"/>
         <v>1216.0000000000007</v>
       </c>
       <c r="R83" s="3">
-        <f t="shared" si="20"/>
+        <f t="shared" si="11"/>
         <v>24.3</v>
       </c>
     </row>
     <row r="84" spans="14:18" x14ac:dyDescent="0.35">
       <c r="N84">
-        <f t="shared" si="21"/>
+        <f t="shared" si="12"/>
         <v>0.77000000000000046</v>
       </c>
       <c r="O84" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="8"/>
         <v>1.5400000000000009</v>
       </c>
       <c r="P84" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="9"/>
         <v>554.40000000000032</v>
       </c>
       <c r="Q84" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="10"/>
         <v>1232.0000000000007</v>
       </c>
       <c r="R84" s="3">
-        <f t="shared" si="20"/>
+        <f t="shared" si="11"/>
         <v>24.6</v>
       </c>
     </row>
     <row r="85" spans="14:18" x14ac:dyDescent="0.35">
       <c r="N85">
-        <f t="shared" si="21"/>
+        <f t="shared" si="12"/>
         <v>0.78000000000000047</v>
       </c>
       <c r="O85" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="8"/>
         <v>1.5600000000000009</v>
       </c>
       <c r="P85" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="9"/>
         <v>561.60000000000036</v>
       </c>
       <c r="Q85" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="10"/>
         <v>1248.0000000000007</v>
       </c>
       <c r="R85" s="3">
-        <f t="shared" si="20"/>
+        <f t="shared" si="11"/>
         <v>25</v>
       </c>
     </row>
     <row r="86" spans="14:18" x14ac:dyDescent="0.35">
       <c r="N86">
-        <f t="shared" si="21"/>
+        <f t="shared" si="12"/>
         <v>0.79000000000000048</v>
       </c>
       <c r="O86" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="8"/>
         <v>1.580000000000001</v>
       </c>
       <c r="P86" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="9"/>
         <v>568.8000000000003</v>
       </c>
       <c r="Q86" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="10"/>
         <v>1264.0000000000007</v>
       </c>
       <c r="R86" s="3">
-        <f t="shared" si="20"/>
+        <f t="shared" si="11"/>
         <v>25.3</v>
       </c>
     </row>
     <row r="87" spans="14:18" x14ac:dyDescent="0.35">
       <c r="N87">
-        <f t="shared" si="21"/>
+        <f t="shared" si="12"/>
         <v>0.80000000000000049</v>
       </c>
       <c r="O87" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="8"/>
         <v>1.600000000000001</v>
       </c>
       <c r="P87" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="9"/>
         <v>576.00000000000034</v>
       </c>
       <c r="Q87" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="10"/>
         <v>1280.0000000000007</v>
       </c>
       <c r="R87" s="3">
-        <f t="shared" si="20"/>
+        <f t="shared" si="11"/>
         <v>25.6</v>
       </c>
     </row>
     <row r="88" spans="14:18" x14ac:dyDescent="0.35">
       <c r="N88">
-        <f t="shared" si="21"/>
+        <f t="shared" si="12"/>
         <v>0.8100000000000005</v>
       </c>
       <c r="O88" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="8"/>
         <v>1.620000000000001</v>
       </c>
       <c r="P88" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="9"/>
         <v>583.20000000000039</v>
       </c>
       <c r="Q88" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="10"/>
         <v>1296.0000000000009</v>
       </c>
       <c r="R88" s="3">
-        <f t="shared" si="20"/>
+        <f t="shared" si="11"/>
         <v>25.9</v>
       </c>
     </row>
     <row r="89" spans="14:18" x14ac:dyDescent="0.35">
       <c r="N89">
-        <f t="shared" si="21"/>
+        <f t="shared" si="12"/>
         <v>0.82000000000000051</v>
       </c>
       <c r="O89" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="8"/>
         <v>1.640000000000001</v>
       </c>
       <c r="P89" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="9"/>
         <v>590.40000000000032</v>
       </c>
       <c r="Q89" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="10"/>
         <v>1312.0000000000009</v>
       </c>
       <c r="R89" s="3">
-        <f t="shared" si="20"/>
+        <f t="shared" si="11"/>
         <v>26.2</v>
       </c>
     </row>
     <row r="90" spans="14:18" x14ac:dyDescent="0.35">
       <c r="N90">
-        <f t="shared" si="21"/>
+        <f t="shared" si="12"/>
         <v>0.83000000000000052</v>
       </c>
       <c r="O90" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="8"/>
         <v>1.660000000000001</v>
       </c>
       <c r="P90" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="9"/>
         <v>597.60000000000036</v>
       </c>
       <c r="Q90" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="10"/>
         <v>1328.0000000000009</v>
       </c>
       <c r="R90" s="3">
-        <f t="shared" si="20"/>
+        <f t="shared" si="11"/>
         <v>26.6</v>
       </c>
     </row>
     <row r="91" spans="14:18" x14ac:dyDescent="0.35">
       <c r="N91">
-        <f t="shared" si="21"/>
+        <f t="shared" si="12"/>
         <v>0.84000000000000052</v>
       </c>
       <c r="O91" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="8"/>
         <v>1.680000000000001</v>
       </c>
       <c r="P91" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="9"/>
         <v>604.80000000000041</v>
       </c>
       <c r="Q91" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="10"/>
         <v>1344.0000000000009</v>
       </c>
       <c r="R91" s="3">
-        <f t="shared" si="20"/>
+        <f t="shared" si="11"/>
         <v>26.9</v>
       </c>
     </row>
     <row r="92" spans="14:18" x14ac:dyDescent="0.35">
       <c r="N92">
-        <f t="shared" si="21"/>
+        <f t="shared" si="12"/>
         <v>0.85000000000000053</v>
       </c>
       <c r="O92" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="8"/>
         <v>1.7000000000000011</v>
       </c>
       <c r="P92" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="9"/>
         <v>612.00000000000034</v>
       </c>
       <c r="Q92" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="10"/>
         <v>1360.0000000000009</v>
       </c>
       <c r="R92" s="3">
-        <f t="shared" si="20"/>
+        <f t="shared" si="11"/>
         <v>27.2</v>
       </c>
     </row>
     <row r="93" spans="14:18" x14ac:dyDescent="0.35">
       <c r="N93">
-        <f t="shared" si="21"/>
+        <f t="shared" si="12"/>
         <v>0.86000000000000054</v>
       </c>
       <c r="O93" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="8"/>
         <v>1.7200000000000011</v>
       </c>
       <c r="P93" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="9"/>
         <v>619.20000000000039</v>
       </c>
       <c r="Q93" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="10"/>
         <v>1376.0000000000009</v>
       </c>
       <c r="R93" s="3">
-        <f t="shared" si="20"/>
+        <f t="shared" si="11"/>
         <v>27.5</v>
       </c>
     </row>
     <row r="94" spans="14:18" x14ac:dyDescent="0.35">
       <c r="N94">
-        <f t="shared" si="21"/>
+        <f t="shared" si="12"/>
         <v>0.87000000000000055</v>
       </c>
       <c r="O94" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="8"/>
         <v>1.7400000000000011</v>
       </c>
       <c r="P94" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="9"/>
         <v>626.40000000000043</v>
       </c>
       <c r="Q94" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="10"/>
         <v>1392.0000000000009</v>
       </c>
       <c r="R94" s="3">
-        <f t="shared" si="20"/>
+        <f t="shared" si="11"/>
         <v>27.8</v>
       </c>
     </row>
     <row r="95" spans="14:18" x14ac:dyDescent="0.35">
       <c r="N95">
-        <f t="shared" si="21"/>
+        <f t="shared" si="12"/>
         <v>0.88000000000000056</v>
       </c>
       <c r="O95" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="8"/>
         <v>1.7600000000000011</v>
       </c>
       <c r="P95" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="9"/>
         <v>633.60000000000036</v>
       </c>
       <c r="Q95" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="10"/>
         <v>1408.0000000000009</v>
       </c>
       <c r="R95" s="3">
-        <f t="shared" si="20"/>
+        <f t="shared" si="11"/>
         <v>28.2</v>
       </c>
     </row>
     <row r="96" spans="14:18" x14ac:dyDescent="0.35">
       <c r="N96">
-        <f t="shared" si="21"/>
+        <f t="shared" si="12"/>
         <v>0.89000000000000057</v>
       </c>
       <c r="O96" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="8"/>
         <v>1.7800000000000011</v>
       </c>
       <c r="P96" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="9"/>
         <v>640.80000000000041</v>
       </c>
       <c r="Q96" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="10"/>
         <v>1424.0000000000009</v>
       </c>
       <c r="R96" s="3">
-        <f t="shared" si="20"/>
+        <f t="shared" si="11"/>
         <v>28.5</v>
       </c>
     </row>
     <row r="97" spans="14:18" x14ac:dyDescent="0.35">
       <c r="N97">
-        <f t="shared" si="21"/>
+        <f t="shared" si="12"/>
         <v>0.90000000000000058</v>
       </c>
       <c r="O97" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="8"/>
         <v>1.8000000000000012</v>
       </c>
       <c r="P97" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="9"/>
         <v>648.00000000000045</v>
       </c>
       <c r="Q97" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="10"/>
         <v>1440.0000000000009</v>
       </c>
       <c r="R97" s="3">
-        <f t="shared" si="20"/>
+        <f t="shared" si="11"/>
         <v>28.8</v>
       </c>
     </row>
     <row r="98" spans="14:18" x14ac:dyDescent="0.35">
       <c r="N98">
-        <f t="shared" si="21"/>
+        <f t="shared" si="12"/>
         <v>0.91000000000000059</v>
       </c>
       <c r="O98" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="8"/>
         <v>1.8200000000000012</v>
       </c>
       <c r="P98" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="9"/>
         <v>655.20000000000039</v>
       </c>
       <c r="Q98" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="10"/>
         <v>1456.0000000000009</v>
       </c>
       <c r="R98" s="3">
-        <f t="shared" si="20"/>
+        <f t="shared" si="11"/>
         <v>29.1</v>
       </c>
     </row>
     <row r="99" spans="14:18" x14ac:dyDescent="0.35">
       <c r="N99">
-        <f t="shared" si="21"/>
+        <f t="shared" si="12"/>
         <v>0.9200000000000006</v>
       </c>
       <c r="O99" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="8"/>
         <v>1.8400000000000012</v>
       </c>
       <c r="P99" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="9"/>
         <v>662.40000000000043</v>
       </c>
       <c r="Q99" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="10"/>
         <v>1472.0000000000009</v>
       </c>
       <c r="R99" s="3">
-        <f t="shared" si="20"/>
+        <f t="shared" si="11"/>
         <v>29.4</v>
       </c>
     </row>
     <row r="100" spans="14:18" x14ac:dyDescent="0.35">
       <c r="N100">
-        <f t="shared" si="21"/>
+        <f t="shared" si="12"/>
         <v>0.9300000000000006</v>
       </c>
       <c r="O100" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="8"/>
         <v>1.8600000000000012</v>
       </c>
       <c r="P100" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="9"/>
         <v>669.60000000000048</v>
       </c>
       <c r="Q100" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="10"/>
         <v>1488.0000000000009</v>
       </c>
       <c r="R100" s="3">
-        <f t="shared" si="20"/>
+        <f t="shared" si="11"/>
         <v>29.8</v>
       </c>
     </row>
     <row r="101" spans="14:18" x14ac:dyDescent="0.35">
       <c r="N101">
-        <f t="shared" si="21"/>
+        <f t="shared" si="12"/>
         <v>0.94000000000000061</v>
       </c>
       <c r="O101" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="8"/>
         <v>1.8800000000000012</v>
       </c>
       <c r="P101" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="9"/>
         <v>676.80000000000041</v>
       </c>
       <c r="Q101" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="10"/>
         <v>1504.0000000000009</v>
       </c>
       <c r="R101" s="3">
-        <f t="shared" si="20"/>
+        <f t="shared" si="11"/>
         <v>30.1</v>
       </c>
     </row>
     <row r="102" spans="14:18" x14ac:dyDescent="0.35">
       <c r="N102">
-        <f t="shared" si="21"/>
+        <f t="shared" si="12"/>
         <v>0.95000000000000062</v>
       </c>
       <c r="O102" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="8"/>
         <v>1.9000000000000012</v>
       </c>
       <c r="P102" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="9"/>
         <v>684.00000000000045</v>
       </c>
       <c r="Q102" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="10"/>
         <v>1520.0000000000009</v>
       </c>
       <c r="R102" s="3">
-        <f t="shared" si="20"/>
+        <f t="shared" si="11"/>
         <v>30.4</v>
       </c>
     </row>
     <row r="103" spans="14:18" x14ac:dyDescent="0.35">
       <c r="N103">
-        <f t="shared" si="21"/>
+        <f t="shared" si="12"/>
         <v>0.96000000000000063</v>
       </c>
       <c r="O103" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="8"/>
         <v>1.9200000000000013</v>
       </c>
       <c r="P103" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="9"/>
         <v>691.2000000000005</v>
       </c>
       <c r="Q103" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="10"/>
         <v>1536.0000000000009</v>
       </c>
       <c r="R103" s="3">
-        <f t="shared" si="20"/>
+        <f t="shared" si="11"/>
         <v>30.7</v>
       </c>
     </row>
     <row r="104" spans="14:18" x14ac:dyDescent="0.35">
       <c r="N104">
-        <f t="shared" si="21"/>
+        <f t="shared" si="12"/>
         <v>0.97000000000000064</v>
       </c>
       <c r="O104" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="8"/>
         <v>1.9400000000000013</v>
       </c>
       <c r="P104" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="9"/>
         <v>698.40000000000043</v>
       </c>
       <c r="Q104" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="10"/>
         <v>1552.0000000000009</v>
       </c>
       <c r="R104" s="3">
-        <f t="shared" si="20"/>
+        <f t="shared" si="11"/>
         <v>31</v>
       </c>
     </row>
     <row r="105" spans="14:18" x14ac:dyDescent="0.35">
       <c r="N105">
-        <f t="shared" si="21"/>
+        <f t="shared" si="12"/>
         <v>0.98000000000000065</v>
       </c>
       <c r="O105" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="8"/>
         <v>1.9600000000000013</v>
       </c>
       <c r="P105" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="9"/>
         <v>705.60000000000048</v>
       </c>
       <c r="Q105" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="10"/>
         <v>1568.0000000000011</v>
       </c>
       <c r="R105" s="3">
-        <f t="shared" si="20"/>
+        <f t="shared" si="11"/>
         <v>31.4</v>
       </c>
     </row>
     <row r="106" spans="14:18" x14ac:dyDescent="0.35">
       <c r="N106">
-        <f t="shared" si="21"/>
+        <f t="shared" si="12"/>
         <v>0.99000000000000066</v>
       </c>
       <c r="O106" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="8"/>
         <v>1.9800000000000013</v>
       </c>
       <c r="P106" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="9"/>
         <v>712.80000000000052</v>
       </c>
       <c r="Q106" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="10"/>
         <v>1584.0000000000011</v>
       </c>
       <c r="R106" s="3">
-        <f t="shared" si="20"/>
+        <f t="shared" si="11"/>
         <v>31.7</v>
       </c>
     </row>
     <row r="107" spans="14:18" x14ac:dyDescent="0.35">
       <c r="N107">
-        <f t="shared" si="21"/>
+        <f t="shared" si="12"/>
         <v>1.0000000000000007</v>
       </c>
       <c r="O107" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="8"/>
         <v>2.0000000000000013</v>
       </c>
       <c r="P107" s="3">
-        <f t="shared" si="18"/>
+        <f t="shared" si="9"/>
         <v>720.00000000000045</v>
       </c>
       <c r="Q107" s="3">
-        <f t="shared" si="19"/>
+        <f t="shared" si="10"/>
         <v>1600.0000000000011</v>
       </c>
       <c r="R107" s="3">
-        <f t="shared" si="20"/>
+        <f t="shared" si="11"/>
         <v>32</v>
       </c>
     </row>
@@ -24058,10 +23030,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5A007A2-5769-4496-B3C8-A596DC860C5C}">
   <dimension ref="A1:AF104"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
+    <sheetView topLeftCell="W1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G1" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="AD43" sqref="AD43"/>
+      <selection pane="bottomLeft" activeCell="AA51" sqref="AA51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -24087,7 +23059,7 @@
   <sheetData>
     <row r="1" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B1">
         <v>16000000</v>
@@ -24099,19 +23071,19 @@
         <v>16000000</v>
       </c>
       <c r="F1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="I1" s="10"/>
       <c r="L1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="O1" s="10"/>
       <c r="S1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="V1" s="10"/>
       <c r="Z1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="AA1" s="9"/>
       <c r="AC1" s="10"/>
@@ -24120,7 +23092,7 @@
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B2">
         <v>64</v>
@@ -24135,78 +23107,78 @@
         <v>4</v>
       </c>
       <c r="G2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="H2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="L2" t="s">
         <v>4</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="N2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="O2" s="10" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="P2" s="9" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="Q2" s="11" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="S2" t="s">
         <v>4</v>
       </c>
       <c r="T2" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="U2" t="s">
+        <v>37</v>
+      </c>
+      <c r="V2" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="W2" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="X2" t="s">
         <v>59</v>
-      </c>
-      <c r="U2" t="s">
-        <v>41</v>
-      </c>
-      <c r="V2" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="W2" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="X2" t="s">
-        <v>63</v>
       </c>
       <c r="Z2" t="s">
         <v>4</v>
       </c>
       <c r="AA2" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC2" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD2" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE2" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF2" t="s">
         <v>59</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>41</v>
-      </c>
-      <c r="AC2" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="AD2" s="25" t="s">
-        <v>60</v>
-      </c>
-      <c r="AE2" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B3">
         <v>125</v>
@@ -24397,7 +23369,7 @@
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B5">
         <f>(1/(B1/B2))*B3</f>
@@ -24510,7 +23482,7 @@
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B6">
         <f>0.001/B5</f>
@@ -24721,7 +23693,7 @@
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B8">
         <v>400</v>
@@ -24828,7 +23800,7 @@
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B9">
         <v>180</v>
@@ -32490,10 +31462,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59B66144-F280-4B56-8DCF-44A144338622}">
   <dimension ref="A1:AL305"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="AC55" sqref="AC55"/>
-      <selection pane="bottomLeft" activeCell="AD4" sqref="AD4"/>
+      <selection pane="bottomLeft" activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -32516,41 +31488,41 @@
   <sheetData>
     <row r="1" spans="1:38" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G1" s="42" t="s">
-        <v>62</v>
-      </c>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
-      <c r="K1" s="42" t="s">
-        <v>72</v>
-      </c>
-      <c r="L1" s="42"/>
-      <c r="M1" s="42"/>
-      <c r="N1" s="42"/>
-      <c r="O1" s="42"/>
+        <v>49</v>
+      </c>
+      <c r="G1" s="45" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45" t="s">
+        <v>68</v>
+      </c>
+      <c r="L1" s="45"/>
+      <c r="M1" s="45"/>
+      <c r="N1" s="45"/>
+      <c r="O1" s="45"/>
       <c r="Q1"/>
       <c r="T1"/>
-      <c r="AF1" s="42" t="s">
-        <v>73</v>
-      </c>
-      <c r="AG1" s="42"/>
-      <c r="AH1" s="42"/>
+      <c r="AF1" s="45" t="s">
+        <v>69</v>
+      </c>
+      <c r="AG1" s="45"/>
+      <c r="AH1" s="45"/>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B2">
         <v>10000</v>
@@ -32571,13 +31543,13 @@
         <v>4</v>
       </c>
       <c r="H2" s="23" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="I2" s="21" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="K2" s="31" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="L2" s="32"/>
       <c r="M2" s="35">
@@ -32599,7 +31571,7 @@
         <v>2.5</v>
       </c>
       <c r="U2" s="36" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.35">
@@ -32641,96 +31613,96 @@
         <v>50</v>
       </c>
       <c r="U3" s="36" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="AF3" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="AG3" s="43">
-        <v>1</v>
-      </c>
-      <c r="AH3" s="44"/>
-      <c r="AI3" s="45"/>
-      <c r="AJ3" s="45"/>
+        <v>73</v>
+      </c>
+      <c r="AG3" s="38">
+        <v>1</v>
+      </c>
+      <c r="AH3" s="39"/>
+      <c r="AI3" s="40"/>
+      <c r="AJ3" s="40"/>
       <c r="AK3" s="18"/>
-      <c r="AL3" s="45"/>
+      <c r="AL3" s="40"/>
     </row>
     <row r="4" spans="1:38" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" t="s">
         <v>54</v>
       </c>
-      <c r="B4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="G4" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="E4" t="s">
-        <v>58</v>
-      </c>
-      <c r="G4" s="14" t="s">
-        <v>61</v>
-      </c>
       <c r="H4" s="15" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="I4" s="15" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="J4" s="12"/>
       <c r="K4" s="16" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="L4" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="M4" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="N4" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="O4" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="P4" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q4" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="R4" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="S4" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="T4" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="M4" s="30" t="s">
+      <c r="AF4" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="AG4" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="AH4" s="30" t="s">
         <v>81</v>
       </c>
-      <c r="N4" s="30" t="s">
-        <v>79</v>
-      </c>
-      <c r="O4" s="30" t="s">
+      <c r="AI4" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="AJ4" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="AK4" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="P4" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q4" s="30" t="s">
-        <v>80</v>
-      </c>
-      <c r="R4" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="S4" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="T4" s="30" t="s">
-        <v>70</v>
-      </c>
-      <c r="AF4" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="AG4" s="30" t="s">
-        <v>84</v>
-      </c>
-      <c r="AH4" s="30" t="s">
-        <v>85</v>
-      </c>
-      <c r="AI4" s="30" t="s">
-        <v>74</v>
-      </c>
-      <c r="AJ4" s="30" t="s">
-        <v>86</v>
-      </c>
-      <c r="AK4" s="24" t="s">
-        <v>75</v>
-      </c>
       <c r="AL4" s="30" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.35">
@@ -32806,7 +31778,7 @@
         <v>0</v>
       </c>
       <c r="AI5" s="29">
-        <f t="shared" ref="AH5:AI68" si="2">IF(($I$15*$AF5)&gt;1, ($AF5-$AF4)*1+AI4, ($I$15 /2)*($AF5^2))</f>
+        <f t="shared" ref="AI5" si="2">IF(($I$15*$AF5)&gt;1, ($AF5-$AF4)*1+AI4, ($I$15 /2)*($AF5^2))</f>
         <v>0</v>
       </c>
       <c r="AJ5" s="29">
@@ -32814,11 +31786,11 @@
         <v>0</v>
       </c>
       <c r="AK5">
-        <f t="shared" ref="AK5:AK68" si="3">IF(($I$45*$AF5)&gt;1, ($AF5-$AF4)*1+AK4, ($I$45 /2)*($AF5^2))</f>
+        <f t="shared" ref="AK5" si="3">IF(($I$45*$AF5)&gt;1, ($AF5-$AF4)*1+AK4, ($I$45 /2)*($AF5^2))</f>
         <v>0</v>
       </c>
       <c r="AL5" s="29">
-        <f t="shared" ref="AL5:AL68" si="4">IF(($I$55*$AF5)&gt;1, ($AF5-$AF4)*1+AL4, ($I$55 /2)*($AF5^2))</f>
+        <f t="shared" ref="AL5" si="4">IF(($I$55*$AF5)&gt;1, ($AF5-$AF4)*1+AL4, ($I$55 /2)*($AF5^2))</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>